<commit_message>
changes made in pre-review
</commit_message>
<xml_diff>
--- a/docs/Final Report/test-table.xlsx
+++ b/docs/Final Report/test-table.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cormac\Documents\GitHub\cs-221-group-project\docs\Final Report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="8920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
   <si>
     <r>
       <rPr>
@@ -577,13 +582,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11">
     <font>
       <sz val="12"/>
@@ -653,39 +652,15 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -708,30 +683,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -741,7 +797,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -751,40 +807,593 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="5">
+    <cellStyle name="Heading" xfId="3"/>
+    <cellStyle name="Heading1" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Result2" xfId="3"/>
-    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
-    <cellStyle name="Result" xfId="6"/>
-    <cellStyle name="Currency[0]" xfId="7" builtinId="7"/>
-    <cellStyle name="Heading" xfId="8"/>
-    <cellStyle name="Heading1" xfId="9"/>
+    <cellStyle name="Result" xfId="2"/>
+    <cellStyle name="Result2" xfId="1"/>
   </cellStyles>
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -853,7 +1462,54 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A45:C71" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+  <autoFilter ref="A45:C71"/>
+  <sortState ref="A41:C66">
+    <sortCondition ref="A4:A30"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Test Reference" dataDxfId="20"/>
+    <tableColumn id="2" name="Pass / Fail" dataDxfId="19"/>
+    <tableColumn id="3" name="Comments" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A32:C40" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A32:C40"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Test Reference" dataDxfId="12"/>
+    <tableColumn id="2" name="Pass / Fail" dataDxfId="11"/>
+    <tableColumn id="3" name="Comments" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A9:C24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A9:C24"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Test Reference" dataDxfId="4"/>
+    <tableColumn id="2" name="Pass / Fail" dataDxfId="3"/>
+    <tableColumn id="3" name="Comments" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1151,6 +1807,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1183,552 +1840,611 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:I38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="10.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
     <col min="3" max="3" width="47.875" customWidth="1"/>
-    <col min="4" max="4" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="10.75" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
-    <col min="6" max="6" width="10.7083333333333" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="10.75" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" customWidth="1"/>
+    <col min="8" max="8" width="10.75" customWidth="1"/>
     <col min="9" max="9" width="28.375" customWidth="1"/>
-    <col min="10" max="16384" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36.55" customHeight="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="36.6" customHeight="1"/>
+    <row r="2" spans="1:3" ht="12.95" customHeight="1">
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.95" customHeight="1"/>
+    <row r="5" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="6" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.600000000000001" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="26" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="27" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="28" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="31" spans="1:3" ht="15.6" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="13"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="1:3" ht="14.25">
+      <c r="A36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" ht="14.25">
+      <c r="A37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="1:3" ht="14.25">
+      <c r="A38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25">
+      <c r="A39" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25">
+      <c r="A40" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="15"/>
+    </row>
+    <row r="42" spans="1:3" ht="18.75">
+      <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="12.85" customHeight="1" spans="1:1">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="12.85" customHeight="1" spans="1:9">
-      <c r="A4" s="3" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="14.25">
+      <c r="A46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="B46" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="47" spans="1:3" ht="14.25">
+      <c r="A47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25">
+      <c r="A48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" ht="14.25">
+      <c r="A49" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" ht="14.25">
+      <c r="A50" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" ht="14.25">
+      <c r="A51" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" ht="14.25">
+      <c r="A52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" ht="14.25">
+      <c r="A53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" ht="14.25">
+      <c r="A54" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25">
+      <c r="A55" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" ht="14.25">
+      <c r="A56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" ht="14.25">
+      <c r="A57" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" ht="14.25">
+      <c r="A58" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" ht="14.25">
+      <c r="A59" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" ht="14.25">
+      <c r="A60" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" ht="14.25">
+      <c r="A61" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" ht="14.25">
+      <c r="A62" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.25">
+      <c r="A63" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25">
+      <c r="A64" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.25">
+      <c r="A65" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25">
+      <c r="A66" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.25">
+      <c r="A67" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25">
+      <c r="A68" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C68" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25">
+      <c r="A69" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="G14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="G15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="G16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A19" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="G19" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="C69" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.25">
+      <c r="A70" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="5" t="s">
+    <row r="71" spans="1:3" ht="14.25">
+      <c r="A71" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" ht="18.65" customHeight="1" spans="1:9">
-      <c r="A24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G25" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" ht="15.65" customHeight="1" spans="7:9">
-      <c r="G26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="G28" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="G29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" ht="15.65" customHeight="1" spans="1:9">
-      <c r="A30" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="G30" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" ht="15.65" customHeight="1" spans="1:3">
-      <c r="A31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" ht="15.65" customHeight="1" spans="1:3">
-      <c r="A32" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" ht="15.65" customHeight="1" spans="1:3">
-      <c r="A33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" ht="15.65" customHeight="1" spans="1:3">
-      <c r="A34" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" ht="15.65" customHeight="1" spans="1:3">
-      <c r="A35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="37" spans="8:9">
-      <c r="H37" t="s">
-        <v>71</v>
-      </c>
-      <c r="I37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="8:9">
-      <c r="H38" t="s">
-        <v>73</v>
-      </c>
-      <c r="I38" t="s">
-        <v>74</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>